<commit_message>
Fix PEI dataset linking issue
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-carbon-capture.xlsx
+++ b/premise/data/additional_inventories/lci-carbon-capture.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/Github/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79D415D5-20A1-8348-8410-7999E2D72DE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{824ACB91-3647-0446-8B1F-8A1BDD01002C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31960" yWindow="60" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DAC" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DAC!$A$1:$T$366</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DAC!$A$1:$T$361</definedName>
   </definedNames>
   <calcPr calcId="191029" calcMode="manual"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1315" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1504" uniqueCount="265">
   <si>
     <t>Activity</t>
   </si>
@@ -744,6 +744,96 @@
   </si>
   <si>
     <t>operation. Uncertainty from deJong et al., 2021</t>
+  </si>
+  <si>
+    <t>carbon dioxide, captured at cement production plant, using monoethanolamine</t>
+  </si>
+  <si>
+    <t>carbon dioxide, captured at cement plant</t>
+  </si>
+  <si>
+    <t>Carbon capture using MEA: Main source: Voldsund (2019) - CEMCAP - D4.6 CEMCAP comparative techno-economic analysis. Heat for MEA regeneration now produced with same fuel mix as MEA kiln (not natural gas as in Voldsund). Transport and storage from Premise inventories. 90% CO2 capture efficiency (process+fuel CO2). Source: Amelie Müller, Carina Harpprecht, Romain Sacchi, Ben Maes, Mariësse van Sluisveld, Vassilis Daioglou, Branko Šavija, Bernhard Steubing, Decarbonizing the cement industry: Findings from coupling prospective life cycle assessment of clinker with integrated assessment model scenarios, Journal of Cleaner Production, 2024, https://doi.org/10.1016/j.jclepro.2024.141884.</t>
+  </si>
+  <si>
+    <t>MEA mark-up, lost in reclaimer (1.4 kg MEA/tCO2) CEMCAP - D4.6 CEMCAP comparative techno-economic analysis, p. 26</t>
+  </si>
+  <si>
+    <t>Electricity consumption for fans, pumps and thermal reclaimer (188 MJ/tclk [primary energy], 761 kg CO2/tclk, 0.459 conversion factor primary to secondary energy, 3.6 MJ/kWh) CEMCAP - D4.6 CEMCAP comparative techno-economic analysis, Table 5.3</t>
+  </si>
+  <si>
+    <t>Electricity consumption for cooling water system (123 MJ/tclk [primary energy], 761 kg CO2/tclk, 0.459 conversion factor primary to secondary energy, 3.6 MJ/kWh) CEMCAP - D4.6 CEMCAP comparative techno-economic analysis, Table 5.3</t>
+  </si>
+  <si>
+    <t>market group for tap water</t>
+  </si>
+  <si>
+    <t>Process water mark-up. CEMCAP - D4.6 CEMCAP comparative techno-economic analysis, Table 5.1</t>
+  </si>
+  <si>
+    <t>Spent MEA solvent: Share of airborne emission and solid emissions from Moser 2011</t>
+  </si>
+  <si>
+    <t>Monoethanolamine</t>
+  </si>
+  <si>
+    <t>MEA emissions, rest is regenerated. Share of airborne emission and solid emissions (process: treatment of spent solvent mixture) from Moser 2011</t>
+  </si>
+  <si>
+    <t>Water</t>
+  </si>
+  <si>
+    <t>Steam for MEA regeneration (3.76 MJ/kg CO2, of which 0.11 can be recuberated from waste heat).</t>
+  </si>
+  <si>
+    <t>steam production, as energy carrier, in chemical industry</t>
+  </si>
+  <si>
+    <t>carbon dioxide storage from hard coal, post, pipeline 200km, storage 1000m</t>
+  </si>
+  <si>
+    <t>Amelie Müller, Carina Harpprecht, Romain Sacchi, Ben Maes, Mariësse van Sluisveld, Vassilis Daioglou, Branko Šavija, Bernhard Steubing, Decarbonizing the cement industry: Findings from coupling prospective life cycle assessment of clinker with integrated assessment model scenarios, Journal of Cleaner Production, 2024, https://doi.org/10.1016/j.jclepro.2024.141884.</t>
+  </si>
+  <si>
+    <t>Energy needed for compression and liquefication of CO2 (CPU): (CEMCAP D4.6, table 5.3)</t>
+  </si>
+  <si>
+    <t>SOx removal, needed so that MEA doesn't form amine salts. Stochiometric amount of 1.25 kg NaOH/kg SOx is sufficient (Cempcap 4.6). 0.00035 kg SOx/kg clinker (ecoinvent), 0.828 kg CO2/kg clinker from GCCA data.</t>
+  </si>
+  <si>
+    <t>carbon dioxide, captured at cement production plant, using direct separation</t>
+  </si>
+  <si>
+    <t>Carbon capture using Direct Separation. Main source: LEILAC project https://ec.europa.eu/research/participants/documents/downloadPublic?documentIds=080166e5df29e8fc&amp;appId=PPGMS. 95% capture efficiency of process related emissions.  Source: Amelie Müller, Carina Harpprecht, Romain Sacchi, Ben Maes, Mariësse van Sluisveld, Vassilis Daioglou, Branko Šavija, Bernhard Steubing, Decarbonizing the cement industry: Findings from coupling prospective life cycle assessment of clinker with integrated assessment model scenarios, Journal of Cleaner Production, 2024, https://doi.org/10.1016/j.jclepro.2024.141884.</t>
+  </si>
+  <si>
+    <t>Additional electricity for LEILAC: LEILAC D3.6 Life Cycle Assessment, Table 4-6: 77kWh/t clinker, Table 4-1: 0.558 t process emissions/t clinker</t>
+  </si>
+  <si>
+    <t>carbon dioxide, captured at cement production plant, using oxyfuel</t>
+  </si>
+  <si>
+    <t>Carbon capture with Oxyfuel technology, where fuel combustion happens in Oxygen-CO2-mix instead of air, which creates a cleaner CO2 flue gas stream. Main source: Voldsund (2019) - CEMCAP - D4.6 CEMCAP comparative techno-economic analysis. 90% CO2 capture efficiency (process+fuel CO2). Includes changes in electricity demand due to new kiln design for oxy-process, oxygen production with ASU, CO2 compression and purification, CO2 transport. Excludes changes in Non-CO2 emissions: CPU reduces SOx (99.99%), NOx (99.36%), Hg (100%) and CO (100%). Source: Amelie Müller, Carina Harpprecht, Romain Sacchi, Ben Maes, Mariësse van Sluisveld, Vassilis Daioglou, Branko Šavija, Bernhard Steubing, Decarbonizing the cement industry: Findings from coupling prospective life cycle assessment of clinker with integrated assessment model scenarios, Journal of Cleaner Production, 2024, https://doi.org/10.1016/j.jclepro.2024.141884.</t>
+  </si>
+  <si>
+    <t>stochiometric amount of O2 needed for combustion with pure oxygen. 11% losses due flue gas looping are already included in the ASU process</t>
+  </si>
+  <si>
+    <t>Electricity savings due to equipment changes: additional fans +122 MJ/tclk , electric power generation -182 MJ/tclk with organic rankine cycle, energy savings at Fans, milling, and handling of solids in kiln -62 MJ/tclk, [all in primary energy], 758 kg CO2/tclk, Conversion factor primary to secondary energy 0.459, 3.6 MJ/kWh. Voldsund (2019) - CEMCAP - D4.6 CEMCAP comparative techno-economic analysis, Table 6.3</t>
+  </si>
+  <si>
+    <t>Electricity consumption cooling water system. 59 MJ/tclk [primary energy], 758 kg CO2/tclk, Conversion factor primary to secondary energy 0.459, 3.6 MJ/kWh. Voldsund (2019) - CEMCAP - D4.6 CEMCAP comparative techno-economic analysis, Table 6.3</t>
+  </si>
+  <si>
+    <t>Compression and purification: Electricity for CPU (440 KJ/kgCO2) (CEMCAP D4.6, table 6.1)</t>
+  </si>
+  <si>
+    <t>industrial gases production, cryogenic air separation</t>
+  </si>
+  <si>
+    <t>oxygen, liquid</t>
+  </si>
+  <si>
+    <t>Compression and purification unit: Electricity for cooling system (0.03 KJ/kg CO2) (CEMCAP D4.6, table 6.1)</t>
   </si>
 </sst>
 </file>
@@ -751,15 +841,15 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="7">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="164" formatCode="0.0E+00"/>
-    <numFmt numFmtId="165" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="166" formatCode="_ * #,##0.000_ ;_ * \-#,##0.000_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="167" formatCode="0.000"/>
-    <numFmt numFmtId="168" formatCode="0.0000"/>
-    <numFmt numFmtId="174" formatCode="_ * #,##0.0000_ ;_ * \-#,##0.0000_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="165" formatCode="0.0E+00"/>
+    <numFmt numFmtId="166" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="167" formatCode="_ * #,##0.000_ ;_ * \-#,##0.000_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="169" formatCode="0.0000"/>
+    <numFmt numFmtId="170" formatCode="_ * #,##0.0000_ ;_ * \-#,##0.0000_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -841,6 +931,22 @@
       <sz val="12"/>
       <name val="Calibri (Body)"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri (Body)"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -861,13 +967,13 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -877,22 +983,28 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="168" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="11" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1208,19 +1320,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T366"/>
+  <dimension ref="A1:T380"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K45" sqref="K45"/>
+    <sheetView tabSelected="1" topLeftCell="A191" workbookViewId="0">
+      <selection activeCell="C222" sqref="C222"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="79.5" customWidth="1"/>
+    <col min="1" max="1" width="47.33203125" customWidth="1"/>
     <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.33203125" customWidth="1"/>
     <col min="6" max="6" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="53" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.5" customWidth="1"/>
     <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.1640625" bestFit="1" customWidth="1"/>
@@ -1518,7 +1630,7 @@
       <c r="A19" t="s">
         <v>74</v>
       </c>
-      <c r="B19" s="25">
+      <c r="B19" s="24">
         <f>-1*B17</f>
         <v>-4.0000000000000001E-3</v>
       </c>
@@ -1542,7 +1654,7 @@
       <c r="A20" t="s">
         <v>75</v>
       </c>
-      <c r="B20" s="26">
+      <c r="B20" s="25">
         <f>-1*B18</f>
         <v>-3.5000000000000001E-3</v>
       </c>
@@ -1932,7 +2044,7 @@
       <c r="A41" t="s">
         <v>74</v>
       </c>
-      <c r="B41" s="25">
+      <c r="B41" s="24">
         <f>-1*B39</f>
         <v>-4.0000000000000001E-3</v>
       </c>
@@ -1956,7 +2068,7 @@
       <c r="A42" t="s">
         <v>75</v>
       </c>
-      <c r="B42" s="26">
+      <c r="B42" s="25">
         <f>-1*B40</f>
         <v>-3.5000000000000001E-3</v>
       </c>
@@ -3114,7 +3226,7 @@
       <c r="I111">
         <v>5</v>
       </c>
-      <c r="J111" s="24">
+      <c r="J111" s="23">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="K111">
@@ -3352,7 +3464,7 @@
       <c r="A125" t="s">
         <v>19</v>
       </c>
-      <c r="B125" s="23" t="s">
+      <c r="B125" t="s">
         <v>231</v>
       </c>
     </row>
@@ -3705,7 +3817,7 @@
       <c r="A144" t="s">
         <v>19</v>
       </c>
-      <c r="B144" s="23" t="s">
+      <c r="B144" t="s">
         <v>231</v>
       </c>
     </row>
@@ -4346,7 +4458,7 @@
       <c r="A179" t="s">
         <v>19</v>
       </c>
-      <c r="B179" s="23" t="s">
+      <c r="B179" t="s">
         <v>231</v>
       </c>
     </row>
@@ -4875,7 +4987,7 @@
         <v>93</v>
       </c>
       <c r="B217">
-        <f>AVERAGE(K217:L217)</f>
+        <f t="shared" ref="B217:B227" si="0">AVERAGE(K217:L217)</f>
         <v>1.9749999999999999</v>
       </c>
       <c r="C217" t="s">
@@ -4909,7 +5021,7 @@
         <v>85</v>
       </c>
       <c r="B218">
-        <f>AVERAGE(K218:L218)</f>
+        <f t="shared" si="0"/>
         <v>3.1749999999999998</v>
       </c>
       <c r="C218" t="s">
@@ -4928,7 +5040,7 @@
         <v>5</v>
       </c>
       <c r="J218">
-        <f t="shared" ref="J218:J227" si="0">B218</f>
+        <f t="shared" ref="J218:J227" si="1">B218</f>
         <v>3.1749999999999998</v>
       </c>
       <c r="K218">
@@ -4943,7 +5055,7 @@
         <v>94</v>
       </c>
       <c r="B219">
-        <f>AVERAGE(K219:L219)</f>
+        <f t="shared" si="0"/>
         <v>2.59</v>
       </c>
       <c r="C219" t="s">
@@ -4962,7 +5074,7 @@
         <v>5</v>
       </c>
       <c r="J219">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.59</v>
       </c>
       <c r="K219">
@@ -4977,7 +5089,7 @@
         <v>95</v>
       </c>
       <c r="B220">
-        <f>AVERAGE(K220:L220)</f>
+        <f t="shared" si="0"/>
         <v>0.19500000000000001</v>
       </c>
       <c r="C220" t="s">
@@ -4996,7 +5108,7 @@
         <v>5</v>
       </c>
       <c r="J220">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.19500000000000001</v>
       </c>
       <c r="K220">
@@ -5011,11 +5123,11 @@
         <v>94</v>
       </c>
       <c r="B221">
-        <f>AVERAGE(K221:L221)</f>
+        <f t="shared" si="0"/>
         <v>0.19500000000000001</v>
       </c>
       <c r="C221" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="D221" t="s">
         <v>6</v>
@@ -5030,7 +5142,7 @@
         <v>5</v>
       </c>
       <c r="J221">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.19500000000000001</v>
       </c>
       <c r="K221">
@@ -5045,7 +5157,7 @@
         <v>96</v>
       </c>
       <c r="B222">
-        <f>AVERAGE(K222:L222)</f>
+        <f t="shared" si="0"/>
         <v>0.11570000000000008</v>
       </c>
       <c r="C222" t="s">
@@ -5067,7 +5179,7 @@
         <v>5</v>
       </c>
       <c r="J222">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.11570000000000008</v>
       </c>
       <c r="K222">
@@ -5084,7 +5196,7 @@
         <v>97</v>
       </c>
       <c r="B223">
-        <f>AVERAGE(K223:L223)</f>
+        <f t="shared" si="0"/>
         <v>1.3817000000000013</v>
       </c>
       <c r="C223" t="s">
@@ -5106,7 +5218,7 @@
         <v>5</v>
       </c>
       <c r="J223">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.3817000000000013</v>
       </c>
       <c r="K223">
@@ -5123,7 +5235,7 @@
         <v>87</v>
       </c>
       <c r="B224">
-        <f>AVERAGE(K224:L224)</f>
+        <f t="shared" si="0"/>
         <v>14.559999999999999</v>
       </c>
       <c r="C224" t="s">
@@ -5142,7 +5254,7 @@
         <v>5</v>
       </c>
       <c r="J224">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14.559999999999999</v>
       </c>
       <c r="K224">
@@ -5157,7 +5269,7 @@
         <v>35</v>
       </c>
       <c r="B225">
-        <f>AVERAGE(K225:L225)</f>
+        <f t="shared" si="0"/>
         <v>0.34499999999999997</v>
       </c>
       <c r="C225" t="s">
@@ -5176,7 +5288,7 @@
         <v>5</v>
       </c>
       <c r="J225">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.34499999999999997</v>
       </c>
       <c r="K225">
@@ -5191,7 +5303,7 @@
         <v>86</v>
       </c>
       <c r="B226">
-        <f>AVERAGE(K226:L226)</f>
+        <f t="shared" si="0"/>
         <v>7.4749999999999996</v>
       </c>
       <c r="C226" t="s">
@@ -5210,7 +5322,7 @@
         <v>5</v>
       </c>
       <c r="J226">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.4749999999999996</v>
       </c>
       <c r="K226">
@@ -5225,7 +5337,7 @@
         <v>74</v>
       </c>
       <c r="B227">
-        <f>AVERAGE(K227:L227)</f>
+        <f t="shared" si="0"/>
         <v>-1.5</v>
       </c>
       <c r="C227" t="s">
@@ -5244,7 +5356,7 @@
         <v>5</v>
       </c>
       <c r="J227">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-1.5</v>
       </c>
       <c r="K227">
@@ -7181,7 +7293,7 @@
         <v>0.16679850853156178</v>
       </c>
     </row>
-    <row r="321" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A321" t="s">
         <v>32</v>
       </c>
@@ -7231,7 +7343,7 @@
         <v>0.16679850853156178</v>
       </c>
     </row>
-    <row r="322" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A322" t="s">
         <v>35</v>
       </c>
@@ -7281,7 +7393,7 @@
         <v>0.16679850853156178</v>
       </c>
     </row>
-    <row r="323" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A323" t="s">
         <v>195</v>
       </c>
@@ -7332,7 +7444,7 @@
         <v>0.16679850853156178</v>
       </c>
     </row>
-    <row r="324" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A324" s="21" t="s">
         <v>93</v>
       </c>
@@ -7382,36 +7494,845 @@
         <v>0.16679850853156178</v>
       </c>
     </row>
-    <row r="330" spans="1:18" ht="16" x14ac:dyDescent="0.2">
-      <c r="A330" s="1"/>
-      <c r="B330" s="1"/>
-    </row>
-    <row r="337" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A337" s="1"/>
-    </row>
-    <row r="344" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A344" s="1"/>
-      <c r="B344" s="1"/>
-    </row>
-    <row r="346" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="B346" s="2"/>
-    </row>
-    <row r="351" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A351" s="1"/>
-    </row>
-    <row r="353" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A353" s="2"/>
-      <c r="J353" s="2"/>
-    </row>
-    <row r="359" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A359" s="1"/>
-      <c r="B359" s="1"/>
-    </row>
-    <row r="366" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A366" s="1"/>
+    <row r="326" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+      <c r="A326" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B326" s="5" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="327" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A327" t="s">
+        <v>7</v>
+      </c>
+      <c r="B327" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="328" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+      <c r="A328" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B328">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="329" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A329" t="s">
+        <v>2</v>
+      </c>
+      <c r="B329" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="330" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A330" t="s">
+        <v>3</v>
+      </c>
+      <c r="B330" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="331" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A331" t="s">
+        <v>5</v>
+      </c>
+      <c r="B331" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="332" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A332" t="s">
+        <v>19</v>
+      </c>
+      <c r="B332" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="333" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A333" t="s">
+        <v>9</v>
+      </c>
+      <c r="B333" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="334" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A334" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="335" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+      <c r="A335" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B335" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C335" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D335" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E335" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F335" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G335" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H335" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I335" s="5"/>
+      <c r="J335" s="5"/>
+      <c r="K335" s="5"/>
+      <c r="L335" s="5"/>
+      <c r="M335" s="5"/>
+      <c r="N335" s="5"/>
+      <c r="O335" s="5"/>
+      <c r="P335" s="5"/>
+      <c r="Q335" s="5"/>
+      <c r="R335" s="5"/>
+      <c r="S335" s="5"/>
+    </row>
+    <row r="336" spans="1:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A336" s="28" t="str">
+        <f>B326</f>
+        <v>carbon dioxide, captured at cement production plant, using monoethanolamine</v>
+      </c>
+      <c r="B336" s="28">
+        <v>1</v>
+      </c>
+      <c r="C336" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D336" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="F336" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="G336" s="28" t="str">
+        <f>B329</f>
+        <v>carbon dioxide, captured at cement plant</v>
+      </c>
+    </row>
+    <row r="337" spans="1:17" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A337" s="28" t="s">
+        <v>249</v>
+      </c>
+      <c r="B337" s="29">
+        <v>1</v>
+      </c>
+      <c r="C337" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D337" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="F337" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="G337" s="28" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="338" spans="1:17" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A338" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="B338" s="29">
+        <f>1.4/1000</f>
+        <v>1.4E-3</v>
+      </c>
+      <c r="C338" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="D338" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="F338" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="G338" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="H338" s="28" t="s">
+        <v>238</v>
+      </c>
+      <c r="N338" s="29"/>
+    </row>
+    <row r="339" spans="1:17" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A339" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="B339" s="29">
+        <f>0.000355*1.25*(1/0.828)</f>
+        <v>5.3592995169082129E-4</v>
+      </c>
+      <c r="C339" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="D339" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="F339" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="G339" s="28" t="s">
+        <v>146</v>
+      </c>
+      <c r="H339" s="28" t="s">
+        <v>252</v>
+      </c>
+      <c r="N339" s="29"/>
+      <c r="P339" s="29"/>
+    </row>
+    <row r="340" spans="1:17" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A340" s="28" t="s">
+        <v>248</v>
+      </c>
+      <c r="B340" s="29">
+        <f>(3.76-0.11)/0.9</f>
+        <v>4.0555555555555554</v>
+      </c>
+      <c r="C340" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D340" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="F340" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="G340" s="28" t="s">
+        <v>196</v>
+      </c>
+      <c r="H340" s="28" t="s">
+        <v>247</v>
+      </c>
+      <c r="N340" s="29"/>
+    </row>
+    <row r="341" spans="1:17" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A341" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B341" s="29">
+        <f>188/761*0.459/3.6</f>
+        <v>3.1498028909329831E-2</v>
+      </c>
+      <c r="C341" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D341" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="F341" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="G341" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="H341" s="28" t="s">
+        <v>239</v>
+      </c>
+      <c r="N341" s="29"/>
+    </row>
+    <row r="342" spans="1:17" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A342" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B342" s="29">
+        <f>123/761*0.459/3.6</f>
+        <v>2.0607752956636003E-2</v>
+      </c>
+      <c r="C342" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D342" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="F342" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="G342" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="H342" s="28" t="s">
+        <v>240</v>
+      </c>
+      <c r="N342" s="29"/>
+    </row>
+    <row r="343" spans="1:17" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A343" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B343" s="29">
+        <f>575/761*0.459/3.6</f>
+        <v>9.63370565045992E-2</v>
+      </c>
+      <c r="C343" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D343" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="F343" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="G343" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="H343" s="28" t="s">
+        <v>251</v>
+      </c>
+      <c r="N343" s="29"/>
+      <c r="Q343" s="30"/>
+    </row>
+    <row r="344" spans="1:17" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A344" s="28" t="s">
+        <v>241</v>
+      </c>
+      <c r="B344" s="29">
+        <f>0.473</f>
+        <v>0.47299999999999998</v>
+      </c>
+      <c r="C344" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="D344" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="F344" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="G344" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="H344" s="28" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="345" spans="1:17" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A345" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="B345" s="29">
+        <f>-B338*0.227/(0.227+0.006)</f>
+        <v>-1.3639484978540772E-3</v>
+      </c>
+      <c r="C345" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="D345" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="F345" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="G345" s="28" t="s">
+        <v>144</v>
+      </c>
+      <c r="H345" s="28" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="346" spans="1:17" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A346" s="28" t="s">
+        <v>244</v>
+      </c>
+      <c r="B346" s="29">
+        <f>1.4/1000*(0.006/0.227+0.006)</f>
+        <v>4.5404405286343617E-5</v>
+      </c>
+      <c r="D346" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E346" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="F346" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="H346" s="28" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="347" spans="1:17" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A347" s="28" t="s">
+        <v>246</v>
+      </c>
+      <c r="B347" s="29">
+        <f>B344/1000</f>
+        <v>4.7299999999999995E-4</v>
+      </c>
+      <c r="D347" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="E347" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="F347" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="G347" s="29"/>
+    </row>
+    <row r="349" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+      <c r="A349" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B349" s="5" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="350" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A350" t="s">
+        <v>7</v>
+      </c>
+      <c r="B350" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="351" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+      <c r="A351" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B351">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="352" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A352" t="s">
+        <v>2</v>
+      </c>
+      <c r="B352" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="353" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A353" t="s">
+        <v>3</v>
+      </c>
+      <c r="B353" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="354" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A354" t="s">
+        <v>5</v>
+      </c>
+      <c r="B354" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="355" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A355" t="s">
+        <v>19</v>
+      </c>
+      <c r="B355" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="356" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A356" t="s">
+        <v>9</v>
+      </c>
+      <c r="B356" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="357" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A357" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="358" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+      <c r="A358" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B358" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C358" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D358" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E358" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F358" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G358" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H358" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I358" s="5"/>
+      <c r="J358" s="5"/>
+      <c r="K358" s="5"/>
+      <c r="L358" s="5"/>
+      <c r="M358" s="5"/>
+      <c r="N358" s="5"/>
+      <c r="O358" s="5"/>
+      <c r="P358" s="5"/>
+      <c r="Q358" s="5"/>
+      <c r="R358" s="5"/>
+      <c r="S358" s="5"/>
+    </row>
+    <row r="359" spans="1:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A359" s="28" t="str">
+        <f>B349</f>
+        <v>carbon dioxide, captured at cement production plant, using direct separation</v>
+      </c>
+      <c r="B359" s="28">
+        <v>1</v>
+      </c>
+      <c r="C359" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D359" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="F359" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="G359" s="28" t="str">
+        <f>B352</f>
+        <v>carbon dioxide, captured at cement plant</v>
+      </c>
+    </row>
+    <row r="360" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A360" s="28" t="s">
+        <v>249</v>
+      </c>
+      <c r="B360" s="29">
+        <v>1</v>
+      </c>
+      <c r="C360" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D360" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E360" s="28"/>
+      <c r="F360" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="G360" s="28" t="s">
+        <v>249</v>
+      </c>
+      <c r="H360" s="28"/>
+    </row>
+    <row r="361" spans="1:19" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A361" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="B361" s="32">
+        <f>77*1/0.558/1000</f>
+        <v>0.13799283154121864</v>
+      </c>
+      <c r="C361" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="D361" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="F361" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="G361" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="H361" s="26" t="s">
+        <v>255</v>
+      </c>
+      <c r="N361" s="32"/>
+    </row>
+    <row r="364" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+      <c r="A364" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B364" s="5" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="365" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A365" t="s">
+        <v>7</v>
+      </c>
+      <c r="B365" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="366" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+      <c r="A366" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B366">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="367" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A367" t="s">
+        <v>2</v>
+      </c>
+      <c r="B367" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="368" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A368" t="s">
+        <v>3</v>
+      </c>
+      <c r="B368" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="369" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A369" t="s">
+        <v>5</v>
+      </c>
+      <c r="B369" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="370" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A370" t="s">
+        <v>19</v>
+      </c>
+      <c r="B370" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="371" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A371" t="s">
+        <v>9</v>
+      </c>
+      <c r="B371" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="372" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A372" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="373" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+      <c r="A373" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B373" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C373" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D373" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E373" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F373" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G373" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H373" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I373" s="5"/>
+      <c r="J373" s="5"/>
+      <c r="K373" s="5"/>
+      <c r="L373" s="5"/>
+      <c r="M373" s="5"/>
+      <c r="N373" s="5"/>
+      <c r="O373" s="5"/>
+      <c r="P373" s="5"/>
+      <c r="Q373" s="5"/>
+      <c r="R373" s="5"/>
+      <c r="S373" s="5"/>
+    </row>
+    <row r="374" spans="1:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A374" s="28" t="str">
+        <f>B364</f>
+        <v>carbon dioxide, captured at cement production plant, using oxyfuel</v>
+      </c>
+      <c r="B374" s="28">
+        <v>1</v>
+      </c>
+      <c r="C374" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D374" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="F374" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="G374" s="28" t="str">
+        <f>B367</f>
+        <v>carbon dioxide, captured at cement plant</v>
+      </c>
+    </row>
+    <row r="375" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A375" s="28" t="s">
+        <v>249</v>
+      </c>
+      <c r="B375" s="29">
+        <v>1</v>
+      </c>
+      <c r="C375" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D375" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E375" s="28"/>
+      <c r="F375" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="G375" s="28" t="s">
+        <v>249</v>
+      </c>
+      <c r="H375" s="28"/>
+    </row>
+    <row r="376" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A376" t="s">
+        <v>262</v>
+      </c>
+      <c r="B376" s="6">
+        <f>B374*32/44/(1-0.11)</f>
+        <v>0.81716036772216549</v>
+      </c>
+      <c r="C376" t="s">
+        <v>27</v>
+      </c>
+      <c r="D376" t="s">
+        <v>6</v>
+      </c>
+      <c r="F376" t="s">
+        <v>16</v>
+      </c>
+      <c r="G376" t="s">
+        <v>263</v>
+      </c>
+      <c r="H376" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="377" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A377" t="s">
+        <v>35</v>
+      </c>
+      <c r="B377" s="6">
+        <f>(122-182-62)/758*0.459/3.6</f>
+        <v>-2.0521108179419524E-2</v>
+      </c>
+      <c r="C377" t="s">
+        <v>8</v>
+      </c>
+      <c r="D377" t="s">
+        <v>24</v>
+      </c>
+      <c r="F377" t="s">
+        <v>16</v>
+      </c>
+      <c r="G377" t="s">
+        <v>25</v>
+      </c>
+      <c r="H377" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="378" spans="1:19" ht="16.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A378" t="s">
+        <v>35</v>
+      </c>
+      <c r="B378" s="6">
+        <f>59/758*0.459/3.6</f>
+        <v>9.9241424802110813E-3</v>
+      </c>
+      <c r="C378" t="s">
+        <v>8</v>
+      </c>
+      <c r="D378" t="s">
+        <v>24</v>
+      </c>
+      <c r="F378" t="s">
+        <v>16</v>
+      </c>
+      <c r="G378" t="s">
+        <v>25</v>
+      </c>
+      <c r="H378" s="26" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="379" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A379" t="s">
+        <v>35</v>
+      </c>
+      <c r="B379" s="6">
+        <f>440/3600</f>
+        <v>0.12222222222222222</v>
+      </c>
+      <c r="C379" t="s">
+        <v>8</v>
+      </c>
+      <c r="D379" t="s">
+        <v>24</v>
+      </c>
+      <c r="F379" t="s">
+        <v>16</v>
+      </c>
+      <c r="G379" t="s">
+        <v>25</v>
+      </c>
+      <c r="H379" t="s">
+        <v>261</v>
+      </c>
+      <c r="M379" s="27"/>
+      <c r="N379" s="31"/>
+    </row>
+    <row r="380" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A380" t="s">
+        <v>35</v>
+      </c>
+      <c r="B380" s="6">
+        <f>0.03/3600</f>
+        <v>8.3333333333333337E-6</v>
+      </c>
+      <c r="C380" t="s">
+        <v>8</v>
+      </c>
+      <c r="D380" t="s">
+        <v>24</v>
+      </c>
+      <c r="F380" t="s">
+        <v>16</v>
+      </c>
+      <c r="G380" t="s">
+        <v>25</v>
+      </c>
+      <c r="H380" t="s">
+        <v>264</v>
+      </c>
+      <c r="M380" s="27"/>
+      <c r="N380" s="31"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:T366" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:T361" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix oxygen input in cement CCS dataset
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-carbon-capture.xlsx
+++ b/premise/data/additional_inventories/lci-carbon-capture.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/Github/premise/premise/data/additional_inventories/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{824ACB91-3647-0446-8B1F-8A1BDD01002C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{117179F3-9F44-FA47-BEFB-6FE597996E0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DAC" sheetId="1" r:id="rId1"/>
@@ -827,13 +827,13 @@
     <t>Compression and purification: Electricity for CPU (440 KJ/kgCO2) (CEMCAP D4.6, table 6.1)</t>
   </si>
   <si>
-    <t>industrial gases production, cryogenic air separation</t>
-  </si>
-  <si>
     <t>oxygen, liquid</t>
   </si>
   <si>
     <t>Compression and purification unit: Electricity for cooling system (0.03 KJ/kg CO2) (CEMCAP D4.6, table 6.1)</t>
+  </si>
+  <si>
+    <t>market for oxygen, liquid</t>
   </si>
 </sst>
 </file>
@@ -841,13 +841,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="7">
-    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="165" formatCode="0.0E+00"/>
-    <numFmt numFmtId="166" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="167" formatCode="_ * #,##0.000_ ;_ * \-#,##0.000_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="168" formatCode="0.000"/>
-    <numFmt numFmtId="169" formatCode="0.0000"/>
-    <numFmt numFmtId="170" formatCode="_ * #,##0.0000_ ;_ * \-#,##0.0000_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="0.0E+00"/>
+    <numFmt numFmtId="165" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="166" formatCode="_ * #,##0.000_ ;_ * \-#,##0.000_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="168" formatCode="0.0000"/>
+    <numFmt numFmtId="169" formatCode="_ * #,##0.0000_ ;_ * \-#,##0.0000_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="15" x14ac:knownFonts="1">
     <font>
@@ -967,13 +967,13 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -983,27 +983,27 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="168" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -1322,8 +1322,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T380"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A191" workbookViewId="0">
-      <selection activeCell="C222" sqref="C222"/>
+    <sheetView tabSelected="1" topLeftCell="A343" workbookViewId="0">
+      <selection activeCell="G376" sqref="G376"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8209,7 +8209,7 @@
     </row>
     <row r="376" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A376" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="B376" s="6">
         <f>B374*32/44/(1-0.11)</f>
@@ -8225,7 +8225,7 @@
         <v>16</v>
       </c>
       <c r="G376" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H376" t="s">
         <v>258</v>
@@ -8326,7 +8326,7 @@
         <v>25</v>
       </c>
       <c r="H380" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="M380" s="27"/>
       <c r="N380" s="31"/>

</xml_diff>

<commit_message>
Error with land occupation and transformation of DAC plants
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-carbon-capture.xlsx
+++ b/premise/data/additional_inventories/lci-carbon-capture.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/Github/premise/premise/data/additional_inventories/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9E52CA1-7281-5E45-B851-9BE691379FDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD1FDB82-6FC0-C74C-92E2-F50D2142BACF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="37680" yWindow="-660" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DAC" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DAC!$A$1:$T$380</definedName>
   </definedNames>
-  <calcPr calcId="191029" calcMode="manual"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -838,13 +838,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="7">
-    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="165" formatCode="0.0E+00"/>
-    <numFmt numFmtId="166" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="167" formatCode="_ * #,##0.000_ ;_ * \-#,##0.000_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="168" formatCode="0.000"/>
-    <numFmt numFmtId="169" formatCode="0.0000"/>
-    <numFmt numFmtId="170" formatCode="_ * #,##0.0000_ ;_ * \-#,##0.0000_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="0.0E+00"/>
+    <numFmt numFmtId="165" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="166" formatCode="_ * #,##0.000_ ;_ * \-#,##0.000_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="168" formatCode="0.0000"/>
+    <numFmt numFmtId="169" formatCode="_ * #,##0.0000_ ;_ * \-#,##0.0000_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="15" x14ac:knownFonts="1">
     <font>
@@ -964,13 +964,13 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -980,27 +980,27 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="168" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -1319,8 +1319,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T380"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A140" workbookViewId="0">
+      <selection activeCell="B168" sqref="B168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2731,8 +2731,8 @@
         <v>210</v>
       </c>
       <c r="B76">
-        <f>78380/1000000000/20</f>
-        <v>3.9190000000000001E-6</v>
+        <f>78380*20</f>
+        <v>1567600</v>
       </c>
       <c r="D76" t="s">
         <v>211</v>
@@ -2752,8 +2752,8 @@
         <v>213</v>
       </c>
       <c r="B77">
-        <f>78380/1000000000</f>
-        <v>7.8380000000000005E-5</v>
+        <f>78380</f>
+        <v>78380</v>
       </c>
       <c r="D77" t="s">
         <v>214</v>
@@ -2773,8 +2773,8 @@
         <v>217</v>
       </c>
       <c r="B78">
-        <f>78380/1000000000</f>
-        <v>7.8380000000000005E-5</v>
+        <f>78380</f>
+        <v>78380</v>
       </c>
       <c r="D78" t="s">
         <v>214</v>
@@ -4358,8 +4358,8 @@
         <v>210</v>
       </c>
       <c r="B168">
-        <f>7838/100000000/20</f>
-        <v>3.9190000000000001E-6</v>
+        <f>7838*20</f>
+        <v>156760</v>
       </c>
       <c r="D168" t="s">
         <v>211</v>
@@ -4379,8 +4379,8 @@
         <v>213</v>
       </c>
       <c r="B169">
-        <f>7838/100000000</f>
-        <v>7.8380000000000005E-5</v>
+        <f>7838</f>
+        <v>7838</v>
       </c>
       <c r="D169" t="s">
         <v>214</v>
@@ -4400,8 +4400,8 @@
         <v>217</v>
       </c>
       <c r="B170">
-        <f>7838/100000000</f>
-        <v>7.8380000000000005E-5</v>
+        <f>7838</f>
+        <v>7838</v>
       </c>
       <c r="D170" t="s">
         <v>214</v>

</xml_diff>

<commit_message>
Continue remind scenarios integration
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-carbon-capture.xlsx
+++ b/premise/data/additional_inventories/lci-carbon-capture.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10420"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/Github/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FFAD961-D345-2045-BF60-6F35D841A5A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EBF5984-4AF7-0749-88AF-DF179BD6522C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34820" yWindow="-300" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="44800" windowHeight="23000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DAC" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2499" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2585" uniqueCount="319">
   <si>
     <t>Activity</t>
   </si>
@@ -966,6 +966,36 @@
   </si>
   <si>
     <t>carbon dioxide, captured and stored, by land-use change</t>
+  </si>
+  <si>
+    <t>carbon dioxide, captured and stored, from a hydrogen production plant using steam methane reforming of biomethane</t>
+  </si>
+  <si>
+    <t>Hydrogen production from natural gas and biomethane with carbon capture and storage – A techno-environmental analysis. 2020. Antonini et al. https://doi.org/10.1039/D0SE00222D</t>
+  </si>
+  <si>
+    <t>This dataset models the pre-combustion capture and compression of carbon dioxide via aqueous methyl diethanolamine (MDEA) absorption in a steam methane reforming (SMR) plant using biomethane as feedstock. The functional unit is 1 kg of CO₂ captured and compressed to 110 bar, suitable for pipeline transport or geological storage. The dataset includes solvent circulation, regeneration via low-pressure steam, CO₂ dehydration and compression, electricity and cooling requirements, as well as infrastructure amortized over a 25-year plant lifetime with a hydrogen output of 75,000 tonnes per year. It excludes upstream hydrogen production, tail gas combustion, and biomethane generation. The system is modeled for European conditions using attributional life cycle assessment with the ecoinvent v3.5 database (cut-off system model), and simulation results derived from Aspen Plus v8.6. MDEA solvent losses are assumed at 5 g per kg of CO₂ captured, and electricity and steam requirements are based on optimized process performance with a CO₂ capture efficiency of 98%. The dataset supports prospective LCAs of low-carbon or net-negative hydrogen systems, and is consistent with data and assumptions reported in Antonini et al. (2020).</t>
+  </si>
+  <si>
+    <t>For auxiliaries, controls, minor pumping/compression</t>
+  </si>
+  <si>
+    <t>For condensing or cooling (varies by setup)</t>
+  </si>
+  <si>
+    <t>Final compression of captured CO₂ for storage/transport</t>
+  </si>
+  <si>
+    <t>MDEA losses from degradation or blowdown</t>
+  </si>
+  <si>
+    <t>Solvent circulation, flue gas fans, CO₂ dehydration</t>
+  </si>
+  <si>
+    <t>Allocation of capital goods per kg CO₂ (25-year life, 75 kt/y plant)</t>
+  </si>
+  <si>
+    <t>Heat recovery &amp; regeneration infrastructure</t>
   </si>
 </sst>
 </file>
@@ -973,13 +1003,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="8">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="164" formatCode="0.0E+00"/>
-    <numFmt numFmtId="165" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="166" formatCode="_ * #,##0.000_ ;_ * \-#,##0.000_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="167" formatCode="0.000"/>
-    <numFmt numFmtId="168" formatCode="0.0000"/>
-    <numFmt numFmtId="169" formatCode="_ * #,##0.0000_ ;_ * \-#,##0.0000_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="165" formatCode="0.0E+00"/>
+    <numFmt numFmtId="166" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="167" formatCode="_ * #,##0.000_ ;_ * \-#,##0.000_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="169" formatCode="0.0000"/>
+    <numFmt numFmtId="170" formatCode="_ * #,##0.0000_ ;_ * \-#,##0.0000_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="171" formatCode="0.00000"/>
   </numFmts>
   <fonts count="15" x14ac:knownFonts="1">
@@ -1100,13 +1130,13 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1116,29 +1146,29 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="168" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1148,12 +1178,10 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="171" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="171" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="171" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1469,10 +1497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V621"/>
+  <dimension ref="A1:V645"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A292" workbookViewId="0">
-      <selection activeCell="B307" sqref="B307"/>
+    <sheetView tabSelected="1" topLeftCell="A613" workbookViewId="0">
+      <selection activeCell="C642" sqref="C642"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8986,7 +9014,7 @@
       <c r="A418" t="s">
         <v>91</v>
       </c>
-      <c r="B418" s="41">
+      <c r="B418" s="38">
         <f t="shared" ref="B418:B428" si="0">AVERAGE(K418:L418)</f>
         <v>1.9749999999999999</v>
       </c>
@@ -10874,7 +10902,7 @@
       <c r="A503" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="B503" s="40">
+      <c r="B503" s="39">
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="C503" s="15" t="s">
@@ -11450,7 +11478,7 @@
       <c r="A525" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="B525" s="39">
+      <c r="B525" s="38">
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="C525" t="s">
@@ -11607,7 +11635,7 @@
         <f>B527</f>
         <v>carbon dioxide, captured, at cement production plant, using monoethanolamine</v>
       </c>
-      <c r="B537" s="38">
+      <c r="B537" s="37">
         <v>1</v>
       </c>
       <c r="C537" s="28" t="s">
@@ -11640,7 +11668,7 @@
       <c r="F538" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="G538" s="37" t="s">
+      <c r="G538" t="s">
         <v>99</v>
       </c>
     </row>
@@ -11648,7 +11676,7 @@
       <c r="A539" s="28" t="s">
         <v>91</v>
       </c>
-      <c r="B539" s="38">
+      <c r="B539" s="37">
         <f>1.4/1000</f>
         <v>1.4E-3</v>
       </c>
@@ -11848,7 +11876,7 @@
       <c r="A547" s="28" t="s">
         <v>234</v>
       </c>
-      <c r="B547" s="42">
+      <c r="B547" s="37">
         <f>1.4/1000*(0.006/0.227+0.006)</f>
         <v>4.5404405286343617E-5</v>
       </c>
@@ -12029,7 +12057,7 @@
       <c r="F561" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="G561" s="37" t="s">
+      <c r="G561" t="s">
         <v>99</v>
       </c>
       <c r="H561" s="28"/>
@@ -12204,7 +12232,7 @@
       <c r="F576" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="G576" s="37" t="s">
+      <c r="G576" t="s">
         <v>99</v>
       </c>
       <c r="H576" s="28"/>
@@ -12613,7 +12641,7 @@
       <c r="A604" t="s">
         <v>234</v>
       </c>
-      <c r="B604" s="41">
+      <c r="B604" s="38">
         <v>6.0000000000000002E-6</v>
       </c>
       <c r="D604" t="s">
@@ -12738,7 +12766,7 @@
       <c r="H608" t="s">
         <v>184</v>
       </c>
-      <c r="I608" s="37" t="s">
+      <c r="I608" t="s">
         <v>99</v>
       </c>
     </row>
@@ -12976,7 +13004,7 @@
       <c r="A617" t="s">
         <v>91</v>
       </c>
-      <c r="B617" s="41">
+      <c r="B617" s="38">
         <v>1.4E-3</v>
       </c>
       <c r="C617" t="s">
@@ -13114,6 +13142,414 @@
       <c r="M621" t="s">
         <v>184</v>
       </c>
+    </row>
+    <row r="623" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+      <c r="A623" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B623" s="1" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="624" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A624" t="s">
+        <v>1</v>
+      </c>
+      <c r="B624">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="625" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A625" t="s">
+        <v>2</v>
+      </c>
+      <c r="B625" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="626" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A626" t="s">
+        <v>3</v>
+      </c>
+      <c r="B626" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="627" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A627" t="s">
+        <v>5</v>
+      </c>
+      <c r="B627" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="628" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A628" t="s">
+        <v>7</v>
+      </c>
+      <c r="B628" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="629" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A629" t="s">
+        <v>18</v>
+      </c>
+      <c r="B629" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="630" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A630" t="s">
+        <v>9</v>
+      </c>
+      <c r="B630" s="40" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="631" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A631" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="632" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A632" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B632" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C632" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D632" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E632" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F632" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G632" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H632" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I632" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="J632" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="K632" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="L632" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="M632" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="633" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A633" t="str">
+        <f>B623</f>
+        <v>carbon dioxide, captured and stored, from a hydrogen production plant using steam methane reforming of biomethane</v>
+      </c>
+      <c r="B633">
+        <v>1</v>
+      </c>
+      <c r="C633" t="s">
+        <v>8</v>
+      </c>
+      <c r="D633" t="s">
+        <v>6</v>
+      </c>
+      <c r="F633" t="s">
+        <v>15</v>
+      </c>
+      <c r="G633" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="634" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A634" t="s">
+        <v>34</v>
+      </c>
+      <c r="B634" s="23">
+        <f>AVERAGE(0.15,0.25)</f>
+        <v>0.2</v>
+      </c>
+      <c r="C634" t="s">
+        <v>8</v>
+      </c>
+      <c r="D634" t="s">
+        <v>23</v>
+      </c>
+      <c r="F634" t="s">
+        <v>16</v>
+      </c>
+      <c r="G634" t="s">
+        <v>24</v>
+      </c>
+      <c r="H634" t="s">
+        <v>312</v>
+      </c>
+      <c r="I634">
+        <v>5</v>
+      </c>
+      <c r="J634" s="23">
+        <f>B634</f>
+        <v>0.2</v>
+      </c>
+      <c r="K634">
+        <v>0.15</v>
+      </c>
+      <c r="L634">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="635" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A635" t="s">
+        <v>31</v>
+      </c>
+      <c r="B635">
+        <f>AVERAGE(1,2)</f>
+        <v>1.5</v>
+      </c>
+      <c r="C635" t="s">
+        <v>132</v>
+      </c>
+      <c r="D635" t="s">
+        <v>6</v>
+      </c>
+      <c r="F635" t="s">
+        <v>16</v>
+      </c>
+      <c r="G635" t="s">
+        <v>32</v>
+      </c>
+      <c r="H635" t="s">
+        <v>313</v>
+      </c>
+      <c r="I635">
+        <v>5</v>
+      </c>
+      <c r="J635" s="23">
+        <f>B635</f>
+        <v>1.5</v>
+      </c>
+      <c r="K635">
+        <v>1</v>
+      </c>
+      <c r="L635">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="636" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A636" t="s">
+        <v>34</v>
+      </c>
+      <c r="B636">
+        <f>AVERAGE(0.1,0.15)</f>
+        <v>0.125</v>
+      </c>
+      <c r="C636" t="s">
+        <v>8</v>
+      </c>
+      <c r="D636" t="s">
+        <v>23</v>
+      </c>
+      <c r="F636" t="s">
+        <v>16</v>
+      </c>
+      <c r="G636" t="s">
+        <v>24</v>
+      </c>
+      <c r="H636" t="s">
+        <v>314</v>
+      </c>
+      <c r="I636">
+        <v>5</v>
+      </c>
+      <c r="J636" s="23">
+        <f>B636</f>
+        <v>0.125</v>
+      </c>
+      <c r="K636">
+        <v>0.1</v>
+      </c>
+      <c r="L636">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="637" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A637" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="B637">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C637" t="s">
+        <v>17</v>
+      </c>
+      <c r="D637" t="s">
+        <v>6</v>
+      </c>
+      <c r="F637" t="s">
+        <v>16</v>
+      </c>
+      <c r="G637" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="H637" t="s">
+        <v>315</v>
+      </c>
+      <c r="I637">
+        <v>5</v>
+      </c>
+      <c r="J637" s="23">
+        <f>B637</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="K637">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="L637">
+        <v>6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="638" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A638" t="s">
+        <v>34</v>
+      </c>
+      <c r="B638">
+        <f>AVERAGE(0.08,0.12)</f>
+        <v>0.1</v>
+      </c>
+      <c r="C638" t="s">
+        <v>8</v>
+      </c>
+      <c r="D638" t="s">
+        <v>23</v>
+      </c>
+      <c r="F638" t="s">
+        <v>16</v>
+      </c>
+      <c r="G638" t="s">
+        <v>24</v>
+      </c>
+      <c r="H638" t="s">
+        <v>316</v>
+      </c>
+      <c r="I638">
+        <v>5</v>
+      </c>
+      <c r="J638" s="23">
+        <f>B638</f>
+        <v>0.1</v>
+      </c>
+      <c r="K638">
+        <v>0.08</v>
+      </c>
+      <c r="L638">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="639" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A639" t="s">
+        <v>42</v>
+      </c>
+      <c r="B639" s="6">
+        <v>1.2E-5</v>
+      </c>
+      <c r="C639" t="s">
+        <v>17</v>
+      </c>
+      <c r="D639" t="s">
+        <v>6</v>
+      </c>
+      <c r="F639" t="s">
+        <v>16</v>
+      </c>
+      <c r="G639" t="s">
+        <v>30</v>
+      </c>
+      <c r="H639" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="640" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A640" t="s">
+        <v>43</v>
+      </c>
+      <c r="B640" s="6">
+        <v>3.9999999999999998E-6</v>
+      </c>
+      <c r="C640" t="s">
+        <v>8</v>
+      </c>
+      <c r="D640" t="s">
+        <v>6</v>
+      </c>
+      <c r="F640" t="s">
+        <v>16</v>
+      </c>
+      <c r="G640" t="s">
+        <v>50</v>
+      </c>
+      <c r="H640" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="641" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A641" t="s">
+        <v>196</v>
+      </c>
+      <c r="B641" s="6">
+        <f>B635*-1/1000</f>
+        <v>-1.5E-3</v>
+      </c>
+      <c r="C641" t="s">
+        <v>132</v>
+      </c>
+      <c r="D641" t="s">
+        <v>49</v>
+      </c>
+      <c r="F641" t="s">
+        <v>16</v>
+      </c>
+      <c r="G641" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="642" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A642" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="B642">
+        <v>1</v>
+      </c>
+      <c r="C642" t="s">
+        <v>8</v>
+      </c>
+      <c r="D642" t="s">
+        <v>6</v>
+      </c>
+      <c r="F642" t="s">
+        <v>16</v>
+      </c>
+      <c r="G642" t="s">
+        <v>99</v>
+      </c>
+      <c r="H642" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="645" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="M645" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:V621" xr:uid="{00000000-0001-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
Continue integration of REMIND scenarios
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-carbon-capture.xlsx
+++ b/premise/data/additional_inventories/lci-carbon-capture.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10420"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/Github/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FFAD961-D345-2045-BF60-6F35D841A5A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EBF5984-4AF7-0749-88AF-DF179BD6522C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34820" yWindow="-300" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="44800" windowHeight="23000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DAC" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2499" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2585" uniqueCount="319">
   <si>
     <t>Activity</t>
   </si>
@@ -966,6 +966,36 @@
   </si>
   <si>
     <t>carbon dioxide, captured and stored, by land-use change</t>
+  </si>
+  <si>
+    <t>carbon dioxide, captured and stored, from a hydrogen production plant using steam methane reforming of biomethane</t>
+  </si>
+  <si>
+    <t>Hydrogen production from natural gas and biomethane with carbon capture and storage – A techno-environmental analysis. 2020. Antonini et al. https://doi.org/10.1039/D0SE00222D</t>
+  </si>
+  <si>
+    <t>This dataset models the pre-combustion capture and compression of carbon dioxide via aqueous methyl diethanolamine (MDEA) absorption in a steam methane reforming (SMR) plant using biomethane as feedstock. The functional unit is 1 kg of CO₂ captured and compressed to 110 bar, suitable for pipeline transport or geological storage. The dataset includes solvent circulation, regeneration via low-pressure steam, CO₂ dehydration and compression, electricity and cooling requirements, as well as infrastructure amortized over a 25-year plant lifetime with a hydrogen output of 75,000 tonnes per year. It excludes upstream hydrogen production, tail gas combustion, and biomethane generation. The system is modeled for European conditions using attributional life cycle assessment with the ecoinvent v3.5 database (cut-off system model), and simulation results derived from Aspen Plus v8.6. MDEA solvent losses are assumed at 5 g per kg of CO₂ captured, and electricity and steam requirements are based on optimized process performance with a CO₂ capture efficiency of 98%. The dataset supports prospective LCAs of low-carbon or net-negative hydrogen systems, and is consistent with data and assumptions reported in Antonini et al. (2020).</t>
+  </si>
+  <si>
+    <t>For auxiliaries, controls, minor pumping/compression</t>
+  </si>
+  <si>
+    <t>For condensing or cooling (varies by setup)</t>
+  </si>
+  <si>
+    <t>Final compression of captured CO₂ for storage/transport</t>
+  </si>
+  <si>
+    <t>MDEA losses from degradation or blowdown</t>
+  </si>
+  <si>
+    <t>Solvent circulation, flue gas fans, CO₂ dehydration</t>
+  </si>
+  <si>
+    <t>Allocation of capital goods per kg CO₂ (25-year life, 75 kt/y plant)</t>
+  </si>
+  <si>
+    <t>Heat recovery &amp; regeneration infrastructure</t>
   </si>
 </sst>
 </file>
@@ -973,13 +1003,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="8">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="164" formatCode="0.0E+00"/>
-    <numFmt numFmtId="165" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="166" formatCode="_ * #,##0.000_ ;_ * \-#,##0.000_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="167" formatCode="0.000"/>
-    <numFmt numFmtId="168" formatCode="0.0000"/>
-    <numFmt numFmtId="169" formatCode="_ * #,##0.0000_ ;_ * \-#,##0.0000_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="165" formatCode="0.0E+00"/>
+    <numFmt numFmtId="166" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="167" formatCode="_ * #,##0.000_ ;_ * \-#,##0.000_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="169" formatCode="0.0000"/>
+    <numFmt numFmtId="170" formatCode="_ * #,##0.0000_ ;_ * \-#,##0.0000_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="171" formatCode="0.00000"/>
   </numFmts>
   <fonts count="15" x14ac:knownFonts="1">
@@ -1100,13 +1130,13 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1116,29 +1146,29 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="168" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1148,12 +1178,10 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="171" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="171" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="171" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1469,10 +1497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V621"/>
+  <dimension ref="A1:V645"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A292" workbookViewId="0">
-      <selection activeCell="B307" sqref="B307"/>
+    <sheetView tabSelected="1" topLeftCell="A613" workbookViewId="0">
+      <selection activeCell="C642" sqref="C642"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8986,7 +9014,7 @@
       <c r="A418" t="s">
         <v>91</v>
       </c>
-      <c r="B418" s="41">
+      <c r="B418" s="38">
         <f t="shared" ref="B418:B428" si="0">AVERAGE(K418:L418)</f>
         <v>1.9749999999999999</v>
       </c>
@@ -10874,7 +10902,7 @@
       <c r="A503" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="B503" s="40">
+      <c r="B503" s="39">
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="C503" s="15" t="s">
@@ -11450,7 +11478,7 @@
       <c r="A525" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="B525" s="39">
+      <c r="B525" s="38">
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="C525" t="s">
@@ -11607,7 +11635,7 @@
         <f>B527</f>
         <v>carbon dioxide, captured, at cement production plant, using monoethanolamine</v>
       </c>
-      <c r="B537" s="38">
+      <c r="B537" s="37">
         <v>1</v>
       </c>
       <c r="C537" s="28" t="s">
@@ -11640,7 +11668,7 @@
       <c r="F538" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="G538" s="37" t="s">
+      <c r="G538" t="s">
         <v>99</v>
       </c>
     </row>
@@ -11648,7 +11676,7 @@
       <c r="A539" s="28" t="s">
         <v>91</v>
       </c>
-      <c r="B539" s="38">
+      <c r="B539" s="37">
         <f>1.4/1000</f>
         <v>1.4E-3</v>
       </c>
@@ -11848,7 +11876,7 @@
       <c r="A547" s="28" t="s">
         <v>234</v>
       </c>
-      <c r="B547" s="42">
+      <c r="B547" s="37">
         <f>1.4/1000*(0.006/0.227+0.006)</f>
         <v>4.5404405286343617E-5</v>
       </c>
@@ -12029,7 +12057,7 @@
       <c r="F561" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="G561" s="37" t="s">
+      <c r="G561" t="s">
         <v>99</v>
       </c>
       <c r="H561" s="28"/>
@@ -12204,7 +12232,7 @@
       <c r="F576" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="G576" s="37" t="s">
+      <c r="G576" t="s">
         <v>99</v>
       </c>
       <c r="H576" s="28"/>
@@ -12613,7 +12641,7 @@
       <c r="A604" t="s">
         <v>234</v>
       </c>
-      <c r="B604" s="41">
+      <c r="B604" s="38">
         <v>6.0000000000000002E-6</v>
       </c>
       <c r="D604" t="s">
@@ -12738,7 +12766,7 @@
       <c r="H608" t="s">
         <v>184</v>
       </c>
-      <c r="I608" s="37" t="s">
+      <c r="I608" t="s">
         <v>99</v>
       </c>
     </row>
@@ -12976,7 +13004,7 @@
       <c r="A617" t="s">
         <v>91</v>
       </c>
-      <c r="B617" s="41">
+      <c r="B617" s="38">
         <v>1.4E-3</v>
       </c>
       <c r="C617" t="s">
@@ -13114,6 +13142,414 @@
       <c r="M621" t="s">
         <v>184</v>
       </c>
+    </row>
+    <row r="623" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+      <c r="A623" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B623" s="1" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="624" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A624" t="s">
+        <v>1</v>
+      </c>
+      <c r="B624">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="625" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A625" t="s">
+        <v>2</v>
+      </c>
+      <c r="B625" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="626" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A626" t="s">
+        <v>3</v>
+      </c>
+      <c r="B626" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="627" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A627" t="s">
+        <v>5</v>
+      </c>
+      <c r="B627" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="628" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A628" t="s">
+        <v>7</v>
+      </c>
+      <c r="B628" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="629" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A629" t="s">
+        <v>18</v>
+      </c>
+      <c r="B629" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="630" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A630" t="s">
+        <v>9</v>
+      </c>
+      <c r="B630" s="40" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="631" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A631" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="632" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A632" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B632" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C632" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D632" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E632" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F632" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G632" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H632" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I632" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="J632" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="K632" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="L632" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="M632" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="633" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A633" t="str">
+        <f>B623</f>
+        <v>carbon dioxide, captured and stored, from a hydrogen production plant using steam methane reforming of biomethane</v>
+      </c>
+      <c r="B633">
+        <v>1</v>
+      </c>
+      <c r="C633" t="s">
+        <v>8</v>
+      </c>
+      <c r="D633" t="s">
+        <v>6</v>
+      </c>
+      <c r="F633" t="s">
+        <v>15</v>
+      </c>
+      <c r="G633" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="634" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A634" t="s">
+        <v>34</v>
+      </c>
+      <c r="B634" s="23">
+        <f>AVERAGE(0.15,0.25)</f>
+        <v>0.2</v>
+      </c>
+      <c r="C634" t="s">
+        <v>8</v>
+      </c>
+      <c r="D634" t="s">
+        <v>23</v>
+      </c>
+      <c r="F634" t="s">
+        <v>16</v>
+      </c>
+      <c r="G634" t="s">
+        <v>24</v>
+      </c>
+      <c r="H634" t="s">
+        <v>312</v>
+      </c>
+      <c r="I634">
+        <v>5</v>
+      </c>
+      <c r="J634" s="23">
+        <f>B634</f>
+        <v>0.2</v>
+      </c>
+      <c r="K634">
+        <v>0.15</v>
+      </c>
+      <c r="L634">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="635" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A635" t="s">
+        <v>31</v>
+      </c>
+      <c r="B635">
+        <f>AVERAGE(1,2)</f>
+        <v>1.5</v>
+      </c>
+      <c r="C635" t="s">
+        <v>132</v>
+      </c>
+      <c r="D635" t="s">
+        <v>6</v>
+      </c>
+      <c r="F635" t="s">
+        <v>16</v>
+      </c>
+      <c r="G635" t="s">
+        <v>32</v>
+      </c>
+      <c r="H635" t="s">
+        <v>313</v>
+      </c>
+      <c r="I635">
+        <v>5</v>
+      </c>
+      <c r="J635" s="23">
+        <f>B635</f>
+        <v>1.5</v>
+      </c>
+      <c r="K635">
+        <v>1</v>
+      </c>
+      <c r="L635">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="636" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A636" t="s">
+        <v>34</v>
+      </c>
+      <c r="B636">
+        <f>AVERAGE(0.1,0.15)</f>
+        <v>0.125</v>
+      </c>
+      <c r="C636" t="s">
+        <v>8</v>
+      </c>
+      <c r="D636" t="s">
+        <v>23</v>
+      </c>
+      <c r="F636" t="s">
+        <v>16</v>
+      </c>
+      <c r="G636" t="s">
+        <v>24</v>
+      </c>
+      <c r="H636" t="s">
+        <v>314</v>
+      </c>
+      <c r="I636">
+        <v>5</v>
+      </c>
+      <c r="J636" s="23">
+        <f>B636</f>
+        <v>0.125</v>
+      </c>
+      <c r="K636">
+        <v>0.1</v>
+      </c>
+      <c r="L636">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="637" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A637" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="B637">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C637" t="s">
+        <v>17</v>
+      </c>
+      <c r="D637" t="s">
+        <v>6</v>
+      </c>
+      <c r="F637" t="s">
+        <v>16</v>
+      </c>
+      <c r="G637" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="H637" t="s">
+        <v>315</v>
+      </c>
+      <c r="I637">
+        <v>5</v>
+      </c>
+      <c r="J637" s="23">
+        <f>B637</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="K637">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="L637">
+        <v>6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="638" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A638" t="s">
+        <v>34</v>
+      </c>
+      <c r="B638">
+        <f>AVERAGE(0.08,0.12)</f>
+        <v>0.1</v>
+      </c>
+      <c r="C638" t="s">
+        <v>8</v>
+      </c>
+      <c r="D638" t="s">
+        <v>23</v>
+      </c>
+      <c r="F638" t="s">
+        <v>16</v>
+      </c>
+      <c r="G638" t="s">
+        <v>24</v>
+      </c>
+      <c r="H638" t="s">
+        <v>316</v>
+      </c>
+      <c r="I638">
+        <v>5</v>
+      </c>
+      <c r="J638" s="23">
+        <f>B638</f>
+        <v>0.1</v>
+      </c>
+      <c r="K638">
+        <v>0.08</v>
+      </c>
+      <c r="L638">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="639" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A639" t="s">
+        <v>42</v>
+      </c>
+      <c r="B639" s="6">
+        <v>1.2E-5</v>
+      </c>
+      <c r="C639" t="s">
+        <v>17</v>
+      </c>
+      <c r="D639" t="s">
+        <v>6</v>
+      </c>
+      <c r="F639" t="s">
+        <v>16</v>
+      </c>
+      <c r="G639" t="s">
+        <v>30</v>
+      </c>
+      <c r="H639" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="640" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A640" t="s">
+        <v>43</v>
+      </c>
+      <c r="B640" s="6">
+        <v>3.9999999999999998E-6</v>
+      </c>
+      <c r="C640" t="s">
+        <v>8</v>
+      </c>
+      <c r="D640" t="s">
+        <v>6</v>
+      </c>
+      <c r="F640" t="s">
+        <v>16</v>
+      </c>
+      <c r="G640" t="s">
+        <v>50</v>
+      </c>
+      <c r="H640" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="641" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A641" t="s">
+        <v>196</v>
+      </c>
+      <c r="B641" s="6">
+        <f>B635*-1/1000</f>
+        <v>-1.5E-3</v>
+      </c>
+      <c r="C641" t="s">
+        <v>132</v>
+      </c>
+      <c r="D641" t="s">
+        <v>49</v>
+      </c>
+      <c r="F641" t="s">
+        <v>16</v>
+      </c>
+      <c r="G641" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="642" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A642" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="B642">
+        <v>1</v>
+      </c>
+      <c r="C642" t="s">
+        <v>8</v>
+      </c>
+      <c r="D642" t="s">
+        <v>6</v>
+      </c>
+      <c r="F642" t="s">
+        <v>16</v>
+      </c>
+      <c r="G642" t="s">
+        <v>99</v>
+      </c>
+      <c r="H642" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="645" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="M645" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:V621" xr:uid="{00000000-0001-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
Update wrt 2.3.0.dev1-steel Adds steel LCIs from Harpprecht et al. 2025
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-carbon-capture.xlsx
+++ b/premise/data/additional_inventories/lci-carbon-capture.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10511"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10720"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D32B30B-2A92-B645-B004-392F8BD1A056}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA28BFAD-10F0-114B-A8B4-C331D85F0120}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34300" yWindow="80" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34920" yWindow="80" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DAC" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2585" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2642" uniqueCount="322">
   <si>
     <t>Activity</t>
   </si>
@@ -996,6 +996,15 @@
   </si>
   <si>
     <t>market for heat, district or industrial, natural gas</t>
+  </si>
+  <si>
+    <t>carbon dioxide, captured and stored, from a biomass fermentation plant</t>
+  </si>
+  <si>
+    <t>Dees J, Oke K, Goldstein H, McCoy ST, Sanchez DL, Simon AJ, Li W. Cost and Life Cycle Emissions of Ethanol Produced with an Oxyfuel Boiler and Carbon Capture and Storage. Environ Sci Technol. 2023 Apr 4;57(13):5391-5403. doi: 10.1021/acs.est.2c04784. Epub 2023 Mar 21. PMID: 36943504; PMCID: PMC10077580.</t>
+  </si>
+  <si>
+    <t>For the fermentation-only CCS (FERMCCS) scenario, Dees et al. performed a full material balance to determine the quantity of CO2 capturable from a 40 M-gal (151 ML) per year ethanol plant. Fermentation CO2 is captured at a rate of 13,089 kg/h and assumed to be at 100% purity. Fermentation CO2 is dehydrated, compressed, liquefied, and pumped at 150 bar, which is assumed to be sufficient to transport the gas by pipeline 100 miles to geologic storage without need for further compression. This is carried out by the CO2 processing unit (CPU) and modeled using Aspen Plus V11. The additional electricity demand for the CPU is estimated to be 110 kWh/t CO2 using this model.</t>
   </si>
 </sst>
 </file>
@@ -1496,10 +1505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V645"/>
+  <dimension ref="A1:V658"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G541" sqref="G541"/>
+    <sheetView tabSelected="1" topLeftCell="A628" workbookViewId="0">
+      <selection activeCell="A612" sqref="A612"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13547,8 +13556,244 @@
         <v>183</v>
       </c>
     </row>
+    <row r="643" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A643" t="s">
+        <v>39</v>
+      </c>
+      <c r="B643">
+        <v>1</v>
+      </c>
+      <c r="D643" t="s">
+        <v>6</v>
+      </c>
+      <c r="E643" t="s">
+        <v>37</v>
+      </c>
+      <c r="F643" t="s">
+        <v>20</v>
+      </c>
+      <c r="G643">
+        <v>0</v>
+      </c>
+      <c r="H643" t="s">
+        <v>284</v>
+      </c>
+      <c r="M643" t="s">
+        <v>183</v>
+      </c>
+    </row>
     <row r="645" spans="1:13" ht="16" x14ac:dyDescent="0.2">
-      <c r="M645" s="2"/>
+      <c r="A645" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B645" s="1" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="646" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A646" t="s">
+        <v>1</v>
+      </c>
+      <c r="B646">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="647" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A647" t="s">
+        <v>2</v>
+      </c>
+      <c r="B647" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="648" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A648" t="s">
+        <v>3</v>
+      </c>
+      <c r="B648" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="649" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A649" t="s">
+        <v>5</v>
+      </c>
+      <c r="B649" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="650" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A650" t="s">
+        <v>7</v>
+      </c>
+      <c r="B650" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="651" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A651" t="s">
+        <v>18</v>
+      </c>
+      <c r="B651" s="6" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="652" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A652" t="s">
+        <v>9</v>
+      </c>
+      <c r="B652" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="653" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A653" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="654" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A654" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B654" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C654" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D654" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E654" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F654" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G654" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H654" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I654" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="J654" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="K654" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="L654" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="M654" s="5" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="655" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A655" t="str">
+        <f>B645</f>
+        <v>carbon dioxide, captured and stored, from a biomass fermentation plant</v>
+      </c>
+      <c r="B655">
+        <v>1</v>
+      </c>
+      <c r="C655" t="s">
+        <v>8</v>
+      </c>
+      <c r="D655" t="s">
+        <v>6</v>
+      </c>
+      <c r="F655" t="s">
+        <v>15</v>
+      </c>
+      <c r="G655" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="656" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A656" t="s">
+        <v>34</v>
+      </c>
+      <c r="B656" s="23">
+        <v>0.11</v>
+      </c>
+      <c r="C656" t="s">
+        <v>8</v>
+      </c>
+      <c r="D656" t="s">
+        <v>23</v>
+      </c>
+      <c r="F656" t="s">
+        <v>16</v>
+      </c>
+      <c r="G656" t="s">
+        <v>24</v>
+      </c>
+      <c r="H656" t="s">
+        <v>311</v>
+      </c>
+      <c r="I656">
+        <v>5</v>
+      </c>
+      <c r="J656" s="23">
+        <f>B656</f>
+        <v>0.11</v>
+      </c>
+      <c r="K656">
+        <v>0.1</v>
+      </c>
+      <c r="L656">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="657" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A657" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="B657">
+        <v>1</v>
+      </c>
+      <c r="C657" t="s">
+        <v>8</v>
+      </c>
+      <c r="D657" t="s">
+        <v>6</v>
+      </c>
+      <c r="F657" t="s">
+        <v>16</v>
+      </c>
+      <c r="G657" t="s">
+        <v>98</v>
+      </c>
+      <c r="H657" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="658" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A658" t="s">
+        <v>39</v>
+      </c>
+      <c r="B658">
+        <v>1</v>
+      </c>
+      <c r="D658" t="s">
+        <v>6</v>
+      </c>
+      <c r="E658" t="s">
+        <v>37</v>
+      </c>
+      <c r="F658" t="s">
+        <v>20</v>
+      </c>
+      <c r="H658" t="s">
+        <v>284</v>
+      </c>
+      <c r="M658" t="s">
+        <v>183</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:V621" xr:uid="{00000000-0001-0000-0000-000000000000}"/>

</xml_diff>